<commit_message>
small changes to finance & weekly report
need remaining time sheets from zayyad, john and steve please.
</commit_message>
<xml_diff>
--- a/Documents/Finance/Financial Summary Report/Business plan - for financial summary.xlsx
+++ b/Documents/Finance/Financial Summary Report/Business plan - for financial summary.xlsx
@@ -331,7 +331,7 @@
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,12 +427,6 @@
       <color indexed="81"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="15">
@@ -811,7 +805,6 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="14" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -828,6 +821,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="38">
     <cellStyle name="40% - Accent4" xfId="2" builtinId="43"/>
@@ -1171,8 +1165,8 @@
   </sheetPr>
   <dimension ref="A1:HA57"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="I2" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView showGridLines="0" topLeftCell="H3" workbookViewId="0">
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1199,57 +1193,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:209" ht="59.25" customHeight="1">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="117" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="118"/>
-      <c r="J1" s="118"/>
-      <c r="K1" s="118"/>
-      <c r="L1" s="118"/>
-      <c r="M1" s="118"/>
-      <c r="N1" s="118"/>
-      <c r="O1" s="118"/>
-      <c r="P1" s="118"/>
-      <c r="Q1" s="118"/>
-      <c r="R1" s="118"/>
-      <c r="S1" s="118"/>
-      <c r="T1" s="118"/>
-      <c r="U1" s="118"/>
-      <c r="V1" s="118"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="117"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+      <c r="Q1" s="117"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
     </row>
     <row r="2" spans="1:209" ht="18">
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
       <c r="G2" s="9"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="115" t="s">
+      <c r="J2" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="115"/>
-      <c r="L2" s="115"/>
-      <c r="M2" s="115"/>
-      <c r="N2" s="115"/>
-      <c r="O2" s="115"/>
-      <c r="P2" s="115"/>
-      <c r="Q2" s="115"/>
-      <c r="R2" s="115"/>
-      <c r="S2" s="115"/>
-      <c r="T2" s="119" t="s">
+      <c r="K2" s="114"/>
+      <c r="L2" s="114"/>
+      <c r="M2" s="114"/>
+      <c r="N2" s="114"/>
+      <c r="O2" s="114"/>
+      <c r="P2" s="114"/>
+      <c r="Q2" s="114"/>
+      <c r="R2" s="114"/>
+      <c r="S2" s="114"/>
+      <c r="T2" s="118" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="119"/>
+      <c r="U2" s="118"/>
       <c r="V2" s="66"/>
       <c r="W2" s="66"/>
       <c r="X2" s="66"/>
@@ -3740,7 +3734,7 @@
       </c>
       <c r="U26" s="106">
         <f>Timesheets!M24</f>
-        <v>350</v>
+        <v>1075</v>
       </c>
       <c r="W26" s="100" t="s">
         <v>54</v>
@@ -4229,12 +4223,12 @@
         <v>3147.5</v>
       </c>
       <c r="T33" s="89">
-        <f t="shared" si="1"/>
+        <f>SUM(T5:T31)</f>
         <v>29800</v>
       </c>
       <c r="U33" s="89">
         <f t="shared" si="1"/>
-        <v>22996.25</v>
+        <v>23721.25</v>
       </c>
       <c r="W33" s="9"/>
       <c r="X33" s="9"/>
@@ -4365,11 +4359,11 @@
     </row>
     <row r="38" spans="1:109">
       <c r="A38" s="3"/>
-      <c r="J38" s="116" t="s">
+      <c r="J38" s="115" t="s">
         <v>38</v>
       </c>
-      <c r="K38" s="116"/>
-      <c r="L38" s="117"/>
+      <c r="K38" s="115"/>
+      <c r="L38" s="116"/>
       <c r="M38" s="92"/>
       <c r="N38" s="94"/>
       <c r="O38" s="17" t="s">
@@ -4437,6 +4431,7 @@
       <c r="P42" s="86" t="s">
         <v>31</v>
       </c>
+      <c r="T42" s="12"/>
     </row>
     <row r="43" spans="1:109">
       <c r="J43" s="98" t="s">
@@ -4531,7 +4526,7 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5372,34 +5367,34 @@
       <c r="B22" s="78">
         <v>3</v>
       </c>
-      <c r="C22" s="104">
-        <v>187.5</v>
-      </c>
-      <c r="D22" s="104">
+      <c r="C22" s="113">
+        <v>187.5</v>
+      </c>
+      <c r="D22" s="113">
         <v>212.5</v>
       </c>
-      <c r="E22" s="104">
+      <c r="E22" s="113">
         <v>62.5</v>
       </c>
-      <c r="F22" s="104">
+      <c r="F22" s="113">
         <v>193.75</v>
       </c>
-      <c r="G22" s="77">
+      <c r="G22" s="113">
         <v>87.5</v>
       </c>
       <c r="H22" s="113">
         <v>0</v>
       </c>
-      <c r="I22" s="114">
+      <c r="I22" s="113">
         <v>100</v>
       </c>
-      <c r="J22" s="77">
+      <c r="J22" s="113">
         <v>137.5</v>
       </c>
-      <c r="K22" s="104">
-        <v>187.5</v>
-      </c>
-      <c r="L22" s="104">
+      <c r="K22" s="113">
+        <v>187.5</v>
+      </c>
+      <c r="L22" s="113">
         <v>137.5</v>
       </c>
       <c r="M22" s="13">
@@ -5414,34 +5409,34 @@
       <c r="B23" s="76">
         <v>4</v>
       </c>
-      <c r="C23" s="104">
+      <c r="C23" s="113">
         <v>137.5</v>
       </c>
-      <c r="D23" s="104">
+      <c r="D23" s="113">
         <v>312.5</v>
       </c>
-      <c r="E23" s="104">
+      <c r="E23" s="113">
         <v>162.5</v>
       </c>
-      <c r="F23" s="104">
+      <c r="F23" s="113">
         <v>200</v>
       </c>
-      <c r="G23" s="104">
+      <c r="G23" s="113">
         <v>162.5</v>
       </c>
-      <c r="H23" s="104">
-        <v>187.5</v>
-      </c>
-      <c r="I23" s="114">
+      <c r="H23" s="113">
+        <v>187.5</v>
+      </c>
+      <c r="I23" s="113">
         <v>100</v>
       </c>
-      <c r="J23" s="104">
+      <c r="J23" s="113">
         <v>125</v>
       </c>
-      <c r="K23" s="104">
+      <c r="K23" s="113">
         <v>237.5</v>
       </c>
-      <c r="L23" s="104">
+      <c r="L23" s="113">
         <v>62.5</v>
       </c>
       <c r="M23" s="13">
@@ -5456,25 +5451,33 @@
       <c r="B24" s="83">
         <v>5</v>
       </c>
-      <c r="C24" s="104"/>
-      <c r="D24" s="104"/>
-      <c r="E24" s="104"/>
-      <c r="F24" s="104"/>
-      <c r="G24" s="104">
-        <v>75</v>
-      </c>
-      <c r="H24" s="104"/>
-      <c r="I24" s="104">
+      <c r="C24" s="113">
+        <v>75</v>
+      </c>
+      <c r="D24" s="113">
+        <v>312.5</v>
+      </c>
+      <c r="E24" s="113">
+        <v>312.5</v>
+      </c>
+      <c r="F24" s="119"/>
+      <c r="G24" s="113">
+        <v>75</v>
+      </c>
+      <c r="H24" s="113">
+        <v>25</v>
+      </c>
+      <c r="I24" s="113">
         <v>112.5</v>
       </c>
-      <c r="J24" s="104"/>
-      <c r="K24" s="104"/>
-      <c r="L24" s="104">
+      <c r="J24" s="119"/>
+      <c r="K24" s="119"/>
+      <c r="L24" s="113">
         <v>162.5</v>
       </c>
       <c r="M24" s="13">
         <f t="shared" si="0"/>
-        <v>350</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -5591,7 +5594,7 @@
       </c>
       <c r="P29" s="12">
         <f>SUM(M20:M29)</f>
-        <v>6000</v>
+        <v>6725</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -5600,15 +5603,15 @@
       </c>
       <c r="C31" s="12">
         <f>SUM(C3:C29)</f>
-        <v>2325</v>
+        <v>2400</v>
       </c>
       <c r="D31" s="12">
         <f>SUM(D3:D29)</f>
-        <v>2837.5</v>
+        <v>3150</v>
       </c>
       <c r="E31" s="12">
         <f>SUM(E3:E29)</f>
-        <v>1937.5</v>
+        <v>2250</v>
       </c>
       <c r="F31" s="12">
         <f t="shared" ref="F31:M31" si="1">SUM(F3:F29)</f>
@@ -5620,7 +5623,7 @@
       </c>
       <c r="H31" s="12">
         <f t="shared" si="1"/>
-        <v>1725</v>
+        <v>1750</v>
       </c>
       <c r="I31" s="12">
         <f t="shared" si="1"/>
@@ -5640,7 +5643,7 @@
       </c>
       <c r="M31" s="107">
         <f t="shared" si="1"/>
-        <v>22996.25</v>
+        <v>23721.25</v>
       </c>
     </row>
     <row r="37" spans="3:13">

</xml_diff>